<commit_message>
Uploaded 20-Oct-2021 19:30:07 {/src/main/resources/com/myspace/eotworkflow/AutoDocGenR.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/myspace/eotworkflow/AutoDocGenR.xlsx
+++ b/src/main/resources/com/myspace/eotworkflow/AutoDocGenR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\212810063\Documents\DTLP\Rotation 1\Drools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBDF6F72-4B68-40C3-A380-9117E379BC95}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03C00036-4BDD-40AA-A7C1-D87A79AECB6B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="610" windowWidth="15510" windowHeight="9590" xr2:uid="{7981FC14-C66D-4D3E-979A-738784BB6AA4}"/>
   </bookViews>
@@ -199,7 +199,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -211,10 +211,7 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -532,8 +529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31998A4C-F8CB-4948-91B9-76A28CCA9776}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -598,11 +595,13 @@
       <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="11"/>
+      <c r="C6" s="10"/>
       <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
@@ -689,7 +688,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B6:F6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Uploaded 20-Oct-2021 19:31:37 {/src/main/resources/com/myspace/eotworkflow/AutoDocGenR.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/myspace/eotworkflow/AutoDocGenR.xlsx
+++ b/src/main/resources/com/myspace/eotworkflow/AutoDocGenR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\212810063\Documents\DTLP\Rotation 1\Drools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03C00036-4BDD-40AA-A7C1-D87A79AECB6B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EE498DE-B882-4DCC-B70D-8A9DCCFC5A3E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="610" windowWidth="15510" windowHeight="9590" xr2:uid="{7981FC14-C66D-4D3E-979A-738784BB6AA4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
   <si>
     <t>RuleSet</t>
   </si>
@@ -61,9 +61,6 @@
   </si>
   <si>
     <t>RULEFLOW-GROUP</t>
-  </si>
-  <si>
-    <t>Case</t>
   </si>
   <si>
     <t>CONDITION</t>
@@ -131,7 +128,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -177,12 +174,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -199,7 +190,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -209,7 +200,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -527,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31998A4C-F8CB-4948-91B9-76A28CCA9776}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -576,48 +566,48 @@
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="4"/>
       <c r="B5" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>8</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
+      <c r="B6" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="D7" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>17</v>
-      </c>
       <c r="F7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
@@ -630,59 +620,52 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>17</v>
+      <c r="F10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" t="s">
         <v>21</v>
       </c>
-      <c r="D11" t="s">
-        <v>22</v>
-      </c>
       <c r="E11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F11" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12" t="s">
-        <v>13</v>
-      </c>
-      <c r="F12" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Uploaded 20-Oct-2021 19:32:19 {/src/main/resources/com/myspace/eotworkflow/AutoDocGenR.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/myspace/eotworkflow/AutoDocGenR.xlsx
+++ b/src/main/resources/com/myspace/eotworkflow/AutoDocGenR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\212810063\Documents\DTLP\Rotation 1\Drools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EE498DE-B882-4DCC-B70D-8A9DCCFC5A3E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C60F2A1B-FBA3-4746-B7A1-5D454D8193EA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="610" windowWidth="15510" windowHeight="9590" xr2:uid="{7981FC14-C66D-4D3E-979A-738784BB6AA4}"/>
   </bookViews>
@@ -34,12 +34,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
   <si>
     <t>RuleSet</t>
-  </si>
-  <si>
-    <t>Sequential</t>
   </si>
   <si>
     <t>RuleTable InvestorApproval</t>
@@ -128,7 +125,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -138,12 +135,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -190,7 +181,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -199,8 +190,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -517,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31998A4C-F8CB-4948-91B9-76A28CCA9776}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -532,146 +522,136 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
-        <v>6</v>
+      <c r="A1" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="3"/>
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="3"/>
+      <c r="B4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="4"/>
-      <c r="B2" s="3" t="s">
+      <c r="B5" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" t="b">
         <v>1</v>
-      </c>
-      <c r="C2" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="D2" s="3"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="4"/>
-      <c r="B4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="4"/>
-      <c r="B5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" t="s">
         <v>20</v>
       </c>
-      <c r="D10" t="s">
-        <v>21</v>
-      </c>
       <c r="E10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F10" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" t="b">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B5:F5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Uploaded 20-Oct-2021 19:33:30 {/src/main/resources/com/myspace/eotworkflow/AutoDocGenR.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/myspace/eotworkflow/AutoDocGenR.xlsx
+++ b/src/main/resources/com/myspace/eotworkflow/AutoDocGenR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\212810063\Documents\DTLP\Rotation 1\Drools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C60F2A1B-FBA3-4746-B7A1-5D454D8193EA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51A997DF-F4D7-4448-A4E6-D3D782DE53E7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="610" windowWidth="15510" windowHeight="9590" xr2:uid="{7981FC14-C66D-4D3E-979A-738784BB6AA4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
   <si>
     <t>RuleSet</t>
   </si>
@@ -52,9 +52,6 @@
   </si>
   <si>
     <t>Notes in this column</t>
-  </si>
-  <si>
-    <t>Descriptions (optional)</t>
   </si>
   <si>
     <t>RULEFLOW-GROUP</t>
@@ -507,10 +504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31998A4C-F8CB-4948-91B9-76A28CCA9776}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B5" sqref="B5:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -546,19 +543,19 @@
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>
       <c r="B4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>8</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
@@ -566,7 +563,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
@@ -578,74 +575,66 @@
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="D6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="F6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="F6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
+      <c r="C7" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="6" t="s">
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>22</v>
+      <c r="F8" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" t="s">
         <v>19</v>
       </c>
-      <c r="D9" t="s">
-        <v>20</v>
-      </c>
       <c r="E9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F9" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Uploaded 20-Oct-2021 19:35:46 {/src/main/resources/com/myspace/eotworkflow/AutoDocGenR.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/myspace/eotworkflow/AutoDocGenR.xlsx
+++ b/src/main/resources/com/myspace/eotworkflow/AutoDocGenR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\212810063\Documents\DTLP\Rotation 1\Drools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51A997DF-F4D7-4448-A4E6-D3D782DE53E7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE7932BD-F598-4799-8264-054A4F43335D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="610" windowWidth="15510" windowHeight="9590" xr2:uid="{7981FC14-C66D-4D3E-979A-738784BB6AA4}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{7981FC14-C66D-4D3E-979A-738784BB6AA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
   <si>
     <t>RuleSet</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>autogen</t>
+  </si>
+  <si>
+    <t>$document</t>
   </si>
 </sst>
 </file>
@@ -166,7 +169,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -174,22 +177,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -507,7 +530,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:F5"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -519,42 +542,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2"/>
+      <c r="D1" s="1"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="3"/>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
     </row>
@@ -567,80 +590,86 @@
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="10" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F6" t="s">
+      <c r="E6" s="6"/>
+      <c r="F6" s="7" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="E7" s="12"/>
+      <c r="F7" s="12" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B8" t="s">
+      <c r="A8" s="13"/>
+      <c r="B8" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="F8" t="b">
+      <c r="F8" s="13" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B9" t="s">
+      <c r="A9" s="13"/>
+      <c r="B9" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="F9" t="b">
+      <c r="F9" s="13" t="b">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B5:D5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Uploaded 20-Oct-2021 19:37:13 {/src/main/resources/com/myspace/eotworkflow/AutoDocGenR.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/myspace/eotworkflow/AutoDocGenR.xlsx
+++ b/src/main/resources/com/myspace/eotworkflow/AutoDocGenR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\212810063\Documents\DTLP\Rotation 1\Drools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE7932BD-F598-4799-8264-054A4F43335D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51E377FC-2C0F-4983-87D2-A44F9198CEC2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{7981FC14-C66D-4D3E-979A-738784BB6AA4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
   <si>
     <t>RuleSet</t>
   </si>
@@ -529,8 +529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31998A4C-F8CB-4948-91B9-76A28CCA9776}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -627,9 +627,7 @@
         <v>14</v>
       </c>
       <c r="E7" s="12"/>
-      <c r="F7" s="12" t="s">
-        <v>21</v>
-      </c>
+      <c r="F7" s="12"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="13"/>

</xml_diff>

<commit_message>
Uploaded 20-Oct-2021 19:38:33 {/src/main/resources/com/myspace/eotworkflow/AutoDocGenR.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/myspace/eotworkflow/AutoDocGenR.xlsx
+++ b/src/main/resources/com/myspace/eotworkflow/AutoDocGenR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\212810063\Documents\DTLP\Rotation 1\Drools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51E377FC-2C0F-4983-87D2-A44F9198CEC2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8060103-CA9B-4806-A7B3-31BFABF0A746}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{7981FC14-C66D-4D3E-979A-738784BB6AA4}"/>
   </bookViews>
@@ -99,10 +99,10 @@
     <t>Bill of Sale</t>
   </si>
   <si>
-    <t>autogen</t>
-  </si>
-  <si>
     <t>$document</t>
+  </si>
+  <si>
+    <t>autogen == $param</t>
   </si>
 </sst>
 </file>
@@ -530,7 +530,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -592,7 +592,7 @@
       <c r="D5" s="8"/>
       <c r="E5" s="9"/>
       <c r="F5" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -610,7 +610,7 @@
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>